<commit_message>
I was a bit slow, the codes that I thaught were missing turned out to be in the HCIMs all along. Added these codes to the profiles, update metadata and display values and fixed and polished everything a bit.
</commit_message>
<xml_diff>
--- a/Mappings/AbilityToDrink - STU3.xlsx
+++ b/Mappings/AbilityToDrink - STU3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edelman\Nictiz-STU3-Zib2017\Mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AAC444-4ECC-4E6C-AD46-E083071A07CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D2B02D-BCC6-4014-B7C8-E69BC9138508}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="157">
   <si>
     <t>Subject</t>
   </si>
@@ -489,9 +489,6 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Observation</t>
-  </si>
-  <si>
     <t>equal</t>
   </si>
   <si>
@@ -504,14 +501,14 @@
     <t>.component, slice .drinkingLimitations</t>
   </si>
   <si>
-    <t>value for .code is missing</t>
+    <t>nl-core-observation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -561,21 +558,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -595,11 +579,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -664,11 +643,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -718,22 +696,15 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Ongeldig" xfId="1" builtinId="27"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7911,7 +7882,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -8346,10 +8317,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="20"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -10911,7 +10882,7 @@
   <dimension ref="B2:T5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11007,14 +10978,12 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
-      <c r="Q3" s="19" t="s">
-        <v>152</v>
+      <c r="Q3" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
-      <c r="T3" s="21" t="s">
-        <v>157</v>
-      </c>
+      <c r="T3" s="4"/>
     </row>
     <row r="4" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B4" s="11"/>
@@ -11050,17 +11019,17 @@
         <v>83</v>
       </c>
       <c r="P4" s="2"/>
-      <c r="Q4" s="20" t="s">
+      <c r="Q4" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="R4" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="S4" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" s="19" t="s">
         <v>154</v>
-      </c>
-      <c r="R4" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="S4" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="T4" s="20" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="5" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
@@ -11097,13 +11066,13 @@
         <v>91</v>
       </c>
       <c r="P5" s="2"/>
-      <c r="Q5" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="R5" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="S5" s="20" t="s">
+      <c r="Q5" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="R5" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="S5" s="19" t="s">
         <v>2</v>
       </c>
       <c r="T5" s="2"/>
@@ -11137,15 +11106,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
@@ -11243,15 +11212,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">

</xml_diff>